<commit_message>
player id logic changed
</commit_message>
<xml_diff>
--- a/public/sample/player_sheet.xlsx
+++ b/public/sample/player_sheet.xlsx
@@ -14,9 +14,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="17">
-  <si>
-    <t>player_id</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="16">
+  <si>
+    <t>mobile_number</t>
   </si>
   <si>
     <t>first_name</t>
@@ -46,7 +46,7 @@
     <t>Right Hand Batsman</t>
   </si>
   <si>
-    <t>Left Arm Offbreak</t>
+    <t>Right Arm Fast</t>
   </si>
   <si>
     <t>Rohit</t>
@@ -62,9 +62,6 @@
   </si>
   <si>
     <t>Bowler</t>
-  </si>
-  <si>
-    <t>Right Arm Fast</t>
   </si>
 </sst>
 </file>
@@ -72,10 +69,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="22">
     <font>
@@ -102,23 +99,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -132,6 +113,53 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="0"/>
       <name val="Calibri"/>
@@ -139,11 +167,18 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -155,21 +190,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FF9C0006"/>
       <name val="Calibri"/>
@@ -177,53 +197,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -237,11 +212,33 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -254,187 +251,187 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -450,10 +447,8 @@
     <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
+      <top/>
+      <bottom style="medium">
         <color theme="4"/>
       </bottom>
       <diagonal/>
@@ -474,11 +469,32 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -498,17 +514,22 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
       <top style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color theme="4"/>
       </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -521,44 +542,20 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
@@ -568,130 +565,130 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="19" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="28" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1027,7 +1024,7 @@
   <dimension ref="A1:AS4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelRow="3"/>
@@ -1125,7 +1122,7 @@
     </row>
     <row r="2" spans="1:6">
       <c r="A2">
-        <v>855115</v>
+        <v>34342</v>
       </c>
       <c r="B2" t="s">
         <v>6</v>
@@ -1180,13 +1177,13 @@
         <v>9</v>
       </c>
       <c r="F4" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>
-  <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F16">
-      <formula1>"Right Arm Fast, Left Arm Fast, Right Arm Legbreak, Left Arm Offbreak"</formula1>
+  <dataValidations count="4">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2 F3 F4">
+      <formula1>"Right Arm Fast,Right Arm Medium Fast,Left Arm Fast,Left Arm Medium Fast,Off Spinner,Leg Spinner"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D16">
       <formula1>"Batsman, Bowler, WK-Batsman, Batting All Rounder, Bowling All Rounder"</formula1>
@@ -1194,6 +1191,9 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E16">
       <formula1>"Right Hand Batsman, Left Handed Batsman"</formula1>
     </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F5:F16">
+      <formula1>"Right Arm Fast, Left Arm Fast, Right Arm Legbreak, Left Arm Offbreak"</formula1>
+    </dataValidation>
   </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>

</xml_diff>